<commit_message>
Turned Down Rebars Experimental Data
</commit_message>
<xml_diff>
--- a/BBT Tests/Axial Deformation vs. Bending Strain.xlsx
+++ b/BBT Tests/Axial Deformation vs. Bending Strain.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="#7" sheetId="3" r:id="rId1"/>
@@ -19,14 +19,16 @@
     <sheet name="No6_CL5" sheetId="5" r:id="rId5"/>
     <sheet name="No6_CL10" sheetId="6" r:id="rId6"/>
     <sheet name="No6_CL15" sheetId="7" r:id="rId7"/>
-    <sheet name="No6_CL20" sheetId="8" r:id="rId8"/>
+    <sheet name="No6_turneddown_bars" sheetId="9" r:id="rId8"/>
+    <sheet name="No6_turneddown_bars (2)" sheetId="10" r:id="rId9"/>
+    <sheet name="No6_CL20" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="32">
   <si>
     <t>Axial Deformation vs. Bending Strain</t>
   </si>
@@ -116,6 +118,12 @@
   </si>
   <si>
     <t>#6 Bar CL=20%</t>
+  </si>
+  <si>
+    <t>Turned down</t>
+  </si>
+  <si>
+    <t>0.5 Bar</t>
   </si>
 </sst>
 </file>
@@ -2651,6 +2659,1485 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:J54"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.7109375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="13" customWidth="1"/>
+    <col min="9" max="10" width="12" style="13" customWidth="1"/>
+    <col min="11" max="32" width="8.7109375" style="14" customWidth="1"/>
+    <col min="33" max="16384" width="14.42578125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+    </row>
+    <row r="2" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="20"/>
+      <c r="C5" s="21">
+        <v>7</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="22"/>
+      <c r="C6" s="23">
+        <v>7.25</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="24">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="25"/>
+      <c r="C8" s="21">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="C9" s="21">
+        <v>-3.1E-2</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="27">
+        <v>0.67082039324993692</v>
+      </c>
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
+    </row>
+    <row r="13" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="61"/>
+    </row>
+    <row r="14" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="55"/>
+      <c r="C14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="30" t="str">
+        <f>+CONCATENATE("L = ",C4,"''")</f>
+        <v>L = 6.5''</v>
+      </c>
+      <c r="I14" s="31" t="str">
+        <f>+CONCATENATE("L = ",C5,"''")</f>
+        <v>L = 7''</v>
+      </c>
+      <c r="J14" s="32" t="str">
+        <f>+CONCATENATE("L = ",C6,"''")</f>
+        <v>L = 7.25''</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="C15" s="6">
+        <f>B15*$C$4/$C$10</f>
+        <v>0.19379255804998177</v>
+      </c>
+      <c r="D15" s="6">
+        <f>B15*$C$5/$C$10</f>
+        <v>0.2086996778999804</v>
+      </c>
+      <c r="E15" s="11">
+        <f>B15*$C$6/$C$10</f>
+        <v>0.21615323782497967</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="H15" s="34">
+        <f>$C$7*C15^2+$C$8*C15+$C$9</f>
+        <v>3.636308493177734E-2</v>
+      </c>
+      <c r="I15" s="35">
+        <f t="shared" ref="I15:J30" si="0">$C$7*D15^2+$C$8*D15+$C$9</f>
+        <v>4.1843527362426886E-2</v>
+      </c>
+      <c r="J15" s="36">
+        <f t="shared" si="0"/>
+        <v>4.4599748577751647E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" ref="C16:C53" si="1">B16*$C$4/$C$10</f>
+        <v>0.29068883707497267</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" ref="D16:D53" si="2">B16*$C$5/$C$10</f>
+        <v>0.31304951684997057</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" ref="E16:E53" si="3">B16*$C$6/$C$10</f>
+        <v>0.32422985673746951</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="37">
+        <v>0.03</v>
+      </c>
+      <c r="H16" s="38">
+        <f t="shared" ref="H16:J53" si="4">$C$7*C16^2+$C$8*C16+$C$9</f>
+        <v>7.2748627397666021E-2</v>
+      </c>
+      <c r="I16" s="39">
+        <f t="shared" si="0"/>
+        <v>8.1401291043640314E-2</v>
+      </c>
+      <c r="J16" s="40">
+        <f t="shared" si="0"/>
+        <v>8.5763622866627476E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="1"/>
+        <v>0.38758511609996354</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="2"/>
+        <v>0.41739935579996079</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="3"/>
+        <v>0.43230647564995933</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="41">
+        <v>0.04</v>
+      </c>
+      <c r="H17" s="34">
+        <f t="shared" si="4"/>
+        <v>0.11093683653022135</v>
+      </c>
+      <c r="I17" s="35">
+        <f t="shared" si="0"/>
+        <v>0.12304972139152046</v>
+      </c>
+      <c r="J17" s="36">
+        <f t="shared" si="0"/>
+        <v>0.12917016382216998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="1"/>
+        <v>0.48448139512495442</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.52174919474995096</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="3"/>
+        <v>0.54038309456244926</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="H18" s="38">
+        <f t="shared" si="4"/>
+        <v>0.15092771232944333</v>
+      </c>
+      <c r="I18" s="39">
+        <f t="shared" si="0"/>
+        <v>0.16678881840606721</v>
+      </c>
+      <c r="J18" s="40">
+        <f t="shared" si="0"/>
+        <v>0.17481937144437917</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="1"/>
+        <v>0.58137767414994534</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" si="2"/>
+        <v>0.62609903369994113</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" si="3"/>
+        <v>0.64845971347493903</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="41">
+        <v>0.06</v>
+      </c>
+      <c r="H19" s="34">
+        <f t="shared" si="4"/>
+        <v>0.19272125479533203</v>
+      </c>
+      <c r="I19" s="35">
+        <f t="shared" si="0"/>
+        <v>0.21261858208728063</v>
+      </c>
+      <c r="J19" s="36">
+        <f t="shared" si="0"/>
+        <v>0.22271124573325493</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="1"/>
+        <v>0.67827395317493633</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" si="2"/>
+        <v>0.73044887264993141</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="3"/>
+        <v>0.7565363323874289</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H20" s="38">
+        <f t="shared" si="4"/>
+        <v>0.23631746392788741</v>
+      </c>
+      <c r="I20" s="39">
+        <f t="shared" si="0"/>
+        <v>0.26053901243516076</v>
+      </c>
+      <c r="J20" s="40">
+        <f t="shared" si="0"/>
+        <v>0.27284578668879744</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="1"/>
+        <v>0.77517023219992709</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="2"/>
+        <v>0.83479871159992158</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="3"/>
+        <v>0.86461295129991866</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="41">
+        <v>0.08</v>
+      </c>
+      <c r="H21" s="34">
+        <f t="shared" si="4"/>
+        <v>0.2817163397271093</v>
+      </c>
+      <c r="I21" s="35">
+        <f t="shared" si="0"/>
+        <v>0.31055010944970751</v>
+      </c>
+      <c r="J21" s="36">
+        <f t="shared" si="0"/>
+        <v>0.32522299431100665</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="1"/>
+        <v>0.87206651122491796</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="2"/>
+        <v>0.93914855054991164</v>
+      </c>
+      <c r="E22" s="11">
+        <f t="shared" si="3"/>
+        <v>0.97268957021240843</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="37">
+        <v>0.09</v>
+      </c>
+      <c r="H22" s="38">
+        <f t="shared" si="4"/>
+        <v>0.328917882192998</v>
+      </c>
+      <c r="I22" s="39">
+        <f t="shared" si="0"/>
+        <v>0.36265187313092095</v>
+      </c>
+      <c r="J22" s="40">
+        <f t="shared" si="0"/>
+        <v>0.37984286859988237</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="1"/>
+        <v>0.96896279024990883</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0434983894999019</v>
+      </c>
+      <c r="E23" s="11">
+        <f t="shared" si="3"/>
+        <v>1.0807661891248985</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="41">
+        <v>0.1</v>
+      </c>
+      <c r="H23" s="34">
+        <f t="shared" si="4"/>
+        <v>0.37792209132555332</v>
+      </c>
+      <c r="I23" s="35">
+        <f t="shared" si="0"/>
+        <v>0.41684430347880108</v>
+      </c>
+      <c r="J23" s="36">
+        <f t="shared" si="0"/>
+        <v>0.43670540955542503</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="1"/>
+        <v>1.0658590692748997</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1478482284498921</v>
+      </c>
+      <c r="E24" s="11">
+        <f t="shared" si="3"/>
+        <v>1.1888428080373881</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="37">
+        <v>0.11</v>
+      </c>
+      <c r="H24" s="38">
+        <f t="shared" si="4"/>
+        <v>0.42872896712477526</v>
+      </c>
+      <c r="I24" s="39">
+        <f t="shared" si="0"/>
+        <v>0.47312740049334778</v>
+      </c>
+      <c r="J24" s="40">
+        <f t="shared" si="0"/>
+        <v>0.49581061717763397</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="1"/>
+        <v>1.1627553482998907</v>
+      </c>
+      <c r="D25" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2521980673998823</v>
+      </c>
+      <c r="E25" s="11">
+        <f t="shared" si="3"/>
+        <v>1.2969194269498781</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="41">
+        <v>0.12</v>
+      </c>
+      <c r="H25" s="34">
+        <f t="shared" si="4"/>
+        <v>0.48133850959066404</v>
+      </c>
+      <c r="I25" s="35">
+        <f t="shared" si="0"/>
+        <v>0.53150116417456117</v>
+      </c>
+      <c r="J25" s="36">
+        <f t="shared" si="0"/>
+        <v>0.55715849146650986</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="8">
+        <v>0.13</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2596516273248815</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3565479063498724</v>
+      </c>
+      <c r="E26" s="11">
+        <f t="shared" si="3"/>
+        <v>1.4049960458623678</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="37">
+        <v>0.13</v>
+      </c>
+      <c r="H26" s="38">
+        <f t="shared" si="4"/>
+        <v>0.53575071872321922</v>
+      </c>
+      <c r="I26" s="39">
+        <f t="shared" si="0"/>
+        <v>0.59196559452244135</v>
+      </c>
+      <c r="J26" s="40">
+        <f t="shared" si="0"/>
+        <v>0.62074903242205237</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3565479063498727</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" si="2"/>
+        <v>1.4608977452998628</v>
+      </c>
+      <c r="E27" s="11">
+        <f t="shared" si="3"/>
+        <v>1.5130726647748578</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="41">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H27" s="34">
+        <f t="shared" si="4"/>
+        <v>0.59196559452244146</v>
+      </c>
+      <c r="I27" s="35">
+        <f t="shared" si="0"/>
+        <v>0.65452069153698822</v>
+      </c>
+      <c r="J27" s="36">
+        <f t="shared" si="0"/>
+        <v>0.6865822400442616</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="1"/>
+        <v>1.4534441853748632</v>
+      </c>
+      <c r="D28" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5652475842498528</v>
+      </c>
+      <c r="E28" s="11">
+        <f t="shared" si="3"/>
+        <v>1.6211492836873473</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="37">
+        <v>0.15</v>
+      </c>
+      <c r="H28" s="38">
+        <f t="shared" si="4"/>
+        <v>0.64998313698832999</v>
+      </c>
+      <c r="I28" s="39">
+        <f t="shared" si="0"/>
+        <v>0.71916645521820166</v>
+      </c>
+      <c r="J28" s="40">
+        <f t="shared" si="0"/>
+        <v>0.75465811433313723</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="1"/>
+        <v>1.5503404643998542</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6695974231998432</v>
+      </c>
+      <c r="E29" s="11">
+        <f t="shared" si="3"/>
+        <v>1.7292259025998373</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="41">
+        <v>0.16</v>
+      </c>
+      <c r="H29" s="34">
+        <f t="shared" si="4"/>
+        <v>0.70980334612088536</v>
+      </c>
+      <c r="I29" s="35">
+        <f t="shared" si="0"/>
+        <v>0.78590288556608179</v>
+      </c>
+      <c r="J29" s="36">
+        <f t="shared" si="0"/>
+        <v>0.82497665528867981</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6472367434248449</v>
+      </c>
+      <c r="D30" s="6">
+        <f t="shared" si="2"/>
+        <v>1.7739472621498333</v>
+      </c>
+      <c r="E30" s="11">
+        <f t="shared" si="3"/>
+        <v>1.8373025215123273</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="37">
+        <v>0.17</v>
+      </c>
+      <c r="H30" s="38">
+        <f t="shared" si="4"/>
+        <v>0.77142622192010724</v>
+      </c>
+      <c r="I30" s="39">
+        <f t="shared" si="0"/>
+        <v>0.8547299825806286</v>
+      </c>
+      <c r="J30" s="40">
+        <f t="shared" si="0"/>
+        <v>0.89753786291088911</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="1"/>
+        <v>1.7441330224498359</v>
+      </c>
+      <c r="D31" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8782971010998233</v>
+      </c>
+      <c r="E31" s="11">
+        <f t="shared" si="3"/>
+        <v>1.9453791404248169</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="H31" s="34">
+        <f t="shared" si="4"/>
+        <v>0.83485176438599595</v>
+      </c>
+      <c r="I31" s="35">
+        <f t="shared" si="4"/>
+        <v>0.92564774626184188</v>
+      </c>
+      <c r="J31" s="36">
+        <f t="shared" si="4"/>
+        <v>0.97234173719976458</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="1"/>
+        <v>1.8410293014748269</v>
+      </c>
+      <c r="D32" s="6">
+        <f t="shared" si="2"/>
+        <v>1.9826469400498137</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" si="3"/>
+        <v>2.0534557593373068</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="37">
+        <v>0.19</v>
+      </c>
+      <c r="H32" s="38">
+        <f t="shared" si="4"/>
+        <v>0.90007997351855151</v>
+      </c>
+      <c r="I32" s="39">
+        <f t="shared" si="4"/>
+        <v>0.99865617660972206</v>
+      </c>
+      <c r="J32" s="40">
+        <f t="shared" si="4"/>
+        <v>1.0493882781553074</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="1"/>
+        <v>1.9379255804998177</v>
+      </c>
+      <c r="D33" s="6">
+        <f t="shared" si="2"/>
+        <v>2.0869967789998038</v>
+      </c>
+      <c r="E33" s="11">
+        <f t="shared" si="3"/>
+        <v>2.161532378249797</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="H33" s="34">
+        <f t="shared" si="4"/>
+        <v>0.96711084931777325</v>
+      </c>
+      <c r="I33" s="35">
+        <f t="shared" si="4"/>
+        <v>1.073755273624269</v>
+      </c>
+      <c r="J33" s="36">
+        <f t="shared" si="4"/>
+        <v>1.1286774857775168</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="1"/>
+        <v>2.0348218595248087</v>
+      </c>
+      <c r="D34" s="6">
+        <f t="shared" si="2"/>
+        <v>2.1913466179497938</v>
+      </c>
+      <c r="E34" s="11">
+        <f t="shared" si="3"/>
+        <v>2.2696089971622864</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="37">
+        <v>0.21</v>
+      </c>
+      <c r="H34" s="38">
+        <f t="shared" si="4"/>
+        <v>1.0359443917836624</v>
+      </c>
+      <c r="I34" s="39">
+        <f t="shared" si="4"/>
+        <v>1.1509450373054821</v>
+      </c>
+      <c r="J34" s="40">
+        <f t="shared" si="4"/>
+        <v>1.2102093600663923</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="1"/>
+        <v>2.1317181385497994</v>
+      </c>
+      <c r="D35" s="6">
+        <f t="shared" si="2"/>
+        <v>2.2956964568997842</v>
+      </c>
+      <c r="E35" s="11">
+        <f t="shared" si="3"/>
+        <v>2.3776856160747761</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="41">
+        <v>0.22</v>
+      </c>
+      <c r="H35" s="34">
+        <f t="shared" si="4"/>
+        <v>1.1065806009162173</v>
+      </c>
+      <c r="I35" s="35">
+        <f t="shared" si="4"/>
+        <v>1.2302254676533624</v>
+      </c>
+      <c r="J35" s="36">
+        <f t="shared" si="4"/>
+        <v>1.2939839010219345</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="1"/>
+        <v>2.2286144175747906</v>
+      </c>
+      <c r="D36" s="6">
+        <f t="shared" si="2"/>
+        <v>2.4000462958497746</v>
+      </c>
+      <c r="E36" s="11">
+        <f t="shared" si="3"/>
+        <v>2.4857622349872663</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="37">
+        <v>0.23</v>
+      </c>
+      <c r="H36" s="38">
+        <f t="shared" si="4"/>
+        <v>1.1790194767154396</v>
+      </c>
+      <c r="I36" s="39">
+        <f t="shared" si="4"/>
+        <v>1.3115965646679093</v>
+      </c>
+      <c r="J36" s="40">
+        <f t="shared" si="4"/>
+        <v>1.3800011086441442</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="1"/>
+        <v>2.3255106965997814</v>
+      </c>
+      <c r="D37" s="6">
+        <f t="shared" si="2"/>
+        <v>2.5043961347997645</v>
+      </c>
+      <c r="E37" s="11">
+        <f t="shared" si="3"/>
+        <v>2.5938388538997561</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="41">
+        <v>0.24</v>
+      </c>
+      <c r="H37" s="34">
+        <f t="shared" si="4"/>
+        <v>1.2532610191813283</v>
+      </c>
+      <c r="I37" s="35">
+        <f t="shared" si="4"/>
+        <v>1.3950583283491225</v>
+      </c>
+      <c r="J37" s="36">
+        <f t="shared" si="4"/>
+        <v>1.46826098293302</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C38" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4224069756247721</v>
+      </c>
+      <c r="D38" s="6">
+        <f t="shared" si="2"/>
+        <v>2.6087459737497545</v>
+      </c>
+      <c r="E38" s="11">
+        <f t="shared" si="3"/>
+        <v>2.7019154728122459</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="37">
+        <v>0.25</v>
+      </c>
+      <c r="H38" s="38">
+        <f t="shared" si="4"/>
+        <v>1.3293052283138835</v>
+      </c>
+      <c r="I38" s="39">
+        <f t="shared" si="4"/>
+        <v>1.4806107586970025</v>
+      </c>
+      <c r="J38" s="40">
+        <f t="shared" si="4"/>
+        <v>1.5587635238885624</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="C39" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5193032546497629</v>
+      </c>
+      <c r="D39" s="6">
+        <f t="shared" si="2"/>
+        <v>2.7130958126997449</v>
+      </c>
+      <c r="E39" s="11">
+        <f t="shared" si="3"/>
+        <v>2.8099920917247356</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="41">
+        <v>0.26</v>
+      </c>
+      <c r="H39" s="34">
+        <f t="shared" si="4"/>
+        <v>1.4071521041131054</v>
+      </c>
+      <c r="I39" s="35">
+        <f t="shared" si="4"/>
+        <v>1.5682538557115495</v>
+      </c>
+      <c r="J39" s="36">
+        <f t="shared" si="4"/>
+        <v>1.6515087315107715</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="C40" s="6">
+        <f t="shared" si="1"/>
+        <v>2.6161995336747541</v>
+      </c>
+      <c r="D40" s="6">
+        <f t="shared" si="2"/>
+        <v>2.8174456516497353</v>
+      </c>
+      <c r="E40" s="11">
+        <f t="shared" si="3"/>
+        <v>2.9180687106372254</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="37">
+        <v>0.27</v>
+      </c>
+      <c r="H40" s="38">
+        <f t="shared" si="4"/>
+        <v>1.4868016465789944</v>
+      </c>
+      <c r="I40" s="39">
+        <f t="shared" si="4"/>
+        <v>1.6579876193927632</v>
+      </c>
+      <c r="J40" s="40">
+        <f t="shared" si="4"/>
+        <v>1.7464966057996472</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C41" s="6">
+        <f t="shared" si="1"/>
+        <v>2.7130958126997453</v>
+      </c>
+      <c r="D41" s="6">
+        <f t="shared" si="2"/>
+        <v>2.9217954905997257</v>
+      </c>
+      <c r="E41" s="11">
+        <f t="shared" si="3"/>
+        <v>3.0261453295497156</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="41">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H41" s="34">
+        <f t="shared" si="4"/>
+        <v>1.5682538557115497</v>
+      </c>
+      <c r="I41" s="35">
+        <f t="shared" si="4"/>
+        <v>1.7498120497406433</v>
+      </c>
+      <c r="J41" s="36">
+        <f t="shared" si="4"/>
+        <v>1.8437271467551901</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C42" s="6">
+        <f t="shared" si="1"/>
+        <v>2.8099920917247352</v>
+      </c>
+      <c r="D42" s="6">
+        <f t="shared" si="2"/>
+        <v>3.0261453295497152</v>
+      </c>
+      <c r="E42" s="11">
+        <f t="shared" si="3"/>
+        <v>3.1342219484622054</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="37">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H42" s="38">
+        <f t="shared" si="4"/>
+        <v>1.651508731510771</v>
+      </c>
+      <c r="I42" s="39">
+        <f t="shared" si="4"/>
+        <v>1.8437271467551897</v>
+      </c>
+      <c r="J42" s="40">
+        <f t="shared" si="4"/>
+        <v>1.943200354377399</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="C43" s="6">
+        <f t="shared" si="1"/>
+        <v>2.9068883707497264</v>
+      </c>
+      <c r="D43" s="6">
+        <f t="shared" si="2"/>
+        <v>3.1304951684997055</v>
+      </c>
+      <c r="E43" s="11">
+        <f t="shared" si="3"/>
+        <v>3.2422985673746947</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="41">
+        <v>0.3</v>
+      </c>
+      <c r="H43" s="34">
+        <f t="shared" si="4"/>
+        <v>1.7365662739766601</v>
+      </c>
+      <c r="I43" s="35">
+        <f t="shared" si="4"/>
+        <v>1.9397329104364034</v>
+      </c>
+      <c r="J43" s="36">
+        <f t="shared" si="4"/>
+        <v>2.0449162286662745</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="C44" s="6">
+        <f t="shared" si="1"/>
+        <v>3.0037846497747176</v>
+      </c>
+      <c r="D44" s="6">
+        <f t="shared" si="2"/>
+        <v>3.2348450074496955</v>
+      </c>
+      <c r="E44" s="11">
+        <f t="shared" si="3"/>
+        <v>3.3503751862871849</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="37">
+        <v>0.31</v>
+      </c>
+      <c r="H44" s="38">
+        <f t="shared" si="4"/>
+        <v>1.8234264831092155</v>
+      </c>
+      <c r="I44" s="39">
+        <f t="shared" si="4"/>
+        <v>2.0378293407842829</v>
+      </c>
+      <c r="J44" s="40">
+        <f t="shared" si="4"/>
+        <v>2.1488747696218171</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="C45" s="6">
+        <f t="shared" si="1"/>
+        <v>3.1006809287997084</v>
+      </c>
+      <c r="D45" s="6">
+        <f t="shared" si="2"/>
+        <v>3.3391948463996863</v>
+      </c>
+      <c r="E45" s="11">
+        <f t="shared" si="3"/>
+        <v>3.4584518051996747</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="41">
+        <v>0.32</v>
+      </c>
+      <c r="H45" s="34">
+        <f t="shared" si="4"/>
+        <v>1.9120893589084376</v>
+      </c>
+      <c r="I45" s="35">
+        <f t="shared" si="4"/>
+        <v>2.13801643779883</v>
+      </c>
+      <c r="J45" s="36">
+        <f t="shared" si="4"/>
+        <v>2.2550759772440263</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="C46" s="6">
+        <f t="shared" si="1"/>
+        <v>3.1975772078246991</v>
+      </c>
+      <c r="D46" s="6">
+        <f t="shared" si="2"/>
+        <v>3.4435446853496763</v>
+      </c>
+      <c r="E46" s="11">
+        <f t="shared" si="3"/>
+        <v>3.5665284241121644</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="37">
+        <v>0.33</v>
+      </c>
+      <c r="H46" s="38">
+        <f t="shared" si="4"/>
+        <v>2.0025549013743258</v>
+      </c>
+      <c r="I46" s="39">
+        <f t="shared" si="4"/>
+        <v>2.2402942014800433</v>
+      </c>
+      <c r="J46" s="40">
+        <f t="shared" si="4"/>
+        <v>2.3635198515329017</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="C47" s="6">
+        <f t="shared" si="1"/>
+        <v>3.2944734868496899</v>
+      </c>
+      <c r="D47" s="6">
+        <f t="shared" si="2"/>
+        <v>3.5478945242996667</v>
+      </c>
+      <c r="E47" s="11">
+        <f t="shared" si="3"/>
+        <v>3.6746050430246546</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="41">
+        <v>0.34</v>
+      </c>
+      <c r="H47" s="34">
+        <f t="shared" si="4"/>
+        <v>2.0948231105068813</v>
+      </c>
+      <c r="I47" s="35">
+        <f t="shared" si="4"/>
+        <v>2.3446626318279242</v>
+      </c>
+      <c r="J47" s="36">
+        <f t="shared" si="4"/>
+        <v>2.4742063924884445</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="C48" s="6">
+        <f t="shared" si="1"/>
+        <v>3.3913697658746806</v>
+      </c>
+      <c r="D48" s="6">
+        <f t="shared" si="2"/>
+        <v>3.6522443632496562</v>
+      </c>
+      <c r="E48" s="11">
+        <f t="shared" si="3"/>
+        <v>3.7826816619371435</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="37">
+        <v>0.35</v>
+      </c>
+      <c r="H48" s="38">
+        <f t="shared" si="4"/>
+        <v>2.1888939863061032</v>
+      </c>
+      <c r="I48" s="39">
+        <f t="shared" si="4"/>
+        <v>2.45112172884247</v>
+      </c>
+      <c r="J48" s="40">
+        <f t="shared" si="4"/>
+        <v>2.5871356001106531</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="C49" s="6">
+        <f t="shared" si="1"/>
+        <v>3.4882660448996718</v>
+      </c>
+      <c r="D49" s="6">
+        <f t="shared" si="2"/>
+        <v>3.7565942021996466</v>
+      </c>
+      <c r="E49" s="11">
+        <f t="shared" si="3"/>
+        <v>3.8907582808496337</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="41">
+        <v>0.36</v>
+      </c>
+      <c r="H49" s="34">
+        <f t="shared" si="4"/>
+        <v>2.284767528771992</v>
+      </c>
+      <c r="I49" s="35">
+        <f t="shared" si="4"/>
+        <v>2.5596714925236834</v>
+      </c>
+      <c r="J49" s="36">
+        <f t="shared" si="4"/>
+        <v>2.7023074743995292</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="8">
+        <v>0.37</v>
+      </c>
+      <c r="C50" s="6">
+        <f t="shared" si="1"/>
+        <v>3.5851623239246626</v>
+      </c>
+      <c r="D50" s="6">
+        <f t="shared" si="2"/>
+        <v>3.8609440411496365</v>
+      </c>
+      <c r="E50" s="11">
+        <f t="shared" si="3"/>
+        <v>3.9988348997621239</v>
+      </c>
+      <c r="G50" s="37">
+        <v>0.37</v>
+      </c>
+      <c r="H50" s="38">
+        <f t="shared" si="4"/>
+        <v>2.3824437379045471</v>
+      </c>
+      <c r="I50" s="39">
+        <f t="shared" si="4"/>
+        <v>2.6703119228715635</v>
+      </c>
+      <c r="J50" s="40">
+        <f t="shared" si="4"/>
+        <v>2.8197220153550719</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="8">
+        <v>0.38</v>
+      </c>
+      <c r="C51" s="6">
+        <f t="shared" si="1"/>
+        <v>3.6820586029496538</v>
+      </c>
+      <c r="D51" s="6">
+        <f t="shared" si="2"/>
+        <v>3.9652938800996274</v>
+      </c>
+      <c r="E51" s="11">
+        <f t="shared" si="3"/>
+        <v>4.1069115186746137</v>
+      </c>
+      <c r="G51" s="41">
+        <v>0.38</v>
+      </c>
+      <c r="H51" s="34">
+        <f t="shared" si="4"/>
+        <v>2.4819226137037695</v>
+      </c>
+      <c r="I51" s="35">
+        <f t="shared" si="4"/>
+        <v>2.7830430198861111</v>
+      </c>
+      <c r="J51" s="36">
+        <f t="shared" si="4"/>
+        <v>2.9393792229772813</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="C52" s="6">
+        <f t="shared" si="1"/>
+        <v>3.7789548819746446</v>
+      </c>
+      <c r="D52" s="6">
+        <f t="shared" si="2"/>
+        <v>4.0696437190496173</v>
+      </c>
+      <c r="E52" s="11">
+        <f t="shared" si="3"/>
+        <v>4.2149881375871034</v>
+      </c>
+      <c r="G52" s="42">
+        <v>0.39</v>
+      </c>
+      <c r="H52" s="38">
+        <f t="shared" si="4"/>
+        <v>2.5832041561696579</v>
+      </c>
+      <c r="I52" s="39">
+        <f t="shared" si="4"/>
+        <v>2.8978647835673246</v>
+      </c>
+      <c r="J52" s="40">
+        <f t="shared" si="4"/>
+        <v>3.0612790972661568</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C53" s="10">
+        <f t="shared" si="1"/>
+        <v>3.8758511609996353</v>
+      </c>
+      <c r="D53" s="10">
+        <f t="shared" si="2"/>
+        <v>4.1739935579996077</v>
+      </c>
+      <c r="E53" s="12">
+        <f t="shared" si="3"/>
+        <v>4.3230647564995941</v>
+      </c>
+      <c r="G53" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="H53" s="44">
+        <f t="shared" si="4"/>
+        <v>2.6862883653022132</v>
+      </c>
+      <c r="I53" s="45">
+        <f t="shared" si="4"/>
+        <v>3.0147772139152047</v>
+      </c>
+      <c r="J53" s="46">
+        <f t="shared" si="4"/>
+        <v>3.1854216382217002</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="G13:J13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J54"/>
@@ -8561,8 +10048,8 @@
   </sheetPr>
   <dimension ref="B1:J54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11520,7 +13007,7 @@
   <dimension ref="B1:J54"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="G12" sqref="G12:J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11556,7 +13043,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11564,7 +13051,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="19">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>10</v>
@@ -11573,7 +13060,7 @@
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20"/>
       <c r="C5" s="21">
-        <v>7</v>
+        <v>7.25</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>11</v>
@@ -11582,7 +13069,7 @@
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22"/>
       <c r="C6" s="23">
-        <v>7.25</v>
+        <v>7.5</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>12</v>
@@ -11624,7 +13111,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="27">
-        <v>0.67082039324993692</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="28"/>
     </row>
@@ -11640,7 +13127,7 @@
       <c r="E12" s="50"/>
       <c r="F12" s="3"/>
       <c r="G12" s="51" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
@@ -11680,15 +13167,15 @@
       </c>
       <c r="H14" s="30" t="str">
         <f>+CONCATENATE("L = ",C4,"''")</f>
-        <v>L = 6.5''</v>
+        <v>L = 7''</v>
       </c>
       <c r="I14" s="31" t="str">
         <f>+CONCATENATE("L = ",C5,"''")</f>
-        <v>L = 7''</v>
+        <v>L = 7.25''</v>
       </c>
       <c r="J14" s="32" t="str">
         <f>+CONCATENATE("L = ",C6,"''")</f>
-        <v>L = 7.25''</v>
+        <v>L = 7.5''</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11697,15 +13184,15 @@
       </c>
       <c r="C15" s="6">
         <f>B15*$C$4/$C$10</f>
-        <v>0.19379255804998177</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D15" s="6">
         <f>B15*$C$5/$C$10</f>
-        <v>0.2086996778999804</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E15" s="11">
         <f>B15*$C$6/$C$10</f>
-        <v>0.21615323782497967</v>
+        <v>0.3</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="33">
@@ -11713,15 +13200,15 @@
       </c>
       <c r="H15" s="34">
         <f>$C$7*C15^2+$C$8*C15+$C$9</f>
-        <v>3.636308493177734E-2</v>
+        <v>6.864640000000001E-2</v>
       </c>
       <c r="I15" s="35">
         <f t="shared" ref="I15:J30" si="0">$C$7*D15^2+$C$8*D15+$C$9</f>
-        <v>4.1843527362426886E-2</v>
+        <v>7.2483599999999995E-2</v>
       </c>
       <c r="J15" s="36">
         <f t="shared" si="0"/>
-        <v>4.4599748577751647E-2</v>
+        <v>7.6339999999999991E-2</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11730,15 +13217,15 @@
       </c>
       <c r="C16" s="6">
         <f t="shared" ref="C16:C53" si="1">B16*$C$4/$C$10</f>
-        <v>0.29068883707497267</v>
+        <v>0.42</v>
       </c>
       <c r="D16" s="6">
         <f t="shared" ref="D16:D53" si="2">B16*$C$5/$C$10</f>
-        <v>0.31304951684997057</v>
+        <v>0.435</v>
       </c>
       <c r="E16" s="11">
         <f t="shared" ref="E16:E53" si="3">B16*$C$6/$C$10</f>
-        <v>0.32422985673746951</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="37">
@@ -11746,15 +13233,15 @@
       </c>
       <c r="H16" s="38">
         <f t="shared" ref="H16:J53" si="4">$C$7*C16^2+$C$8*C16+$C$9</f>
-        <v>7.2748627397666021E-2</v>
+        <v>0.12411439999999999</v>
       </c>
       <c r="I16" s="39">
         <f t="shared" si="0"/>
-        <v>8.1401291043640314E-2</v>
+        <v>0.1302806</v>
       </c>
       <c r="J16" s="40">
         <f t="shared" si="0"/>
-        <v>8.5763622866627476E-2</v>
+        <v>0.13648999999999997</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11763,15 +13250,15 @@
       </c>
       <c r="C17" s="6">
         <f t="shared" si="1"/>
-        <v>0.38758511609996354</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="2"/>
-        <v>0.41739935579996079</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E17" s="11">
         <f t="shared" si="3"/>
-        <v>0.43230647564995933</v>
+        <v>0.6</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="41">
@@ -11779,15 +13266,15 @@
       </c>
       <c r="H17" s="34">
         <f t="shared" si="4"/>
-        <v>0.11093683653022135</v>
+        <v>0.18334560000000003</v>
       </c>
       <c r="I17" s="35">
         <f t="shared" si="0"/>
-        <v>0.12304972139152046</v>
+        <v>0.19211439999999999</v>
       </c>
       <c r="J17" s="36">
         <f t="shared" si="0"/>
-        <v>0.12917016382216998</v>
+        <v>0.20096</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11796,15 +13283,15 @@
       </c>
       <c r="C18" s="6">
         <f t="shared" si="1"/>
-        <v>0.48448139512495442</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="2"/>
-        <v>0.52174919474995096</v>
+        <v>0.72500000000000009</v>
       </c>
       <c r="E18" s="11">
         <f t="shared" si="3"/>
-        <v>0.54038309456244926</v>
+        <v>0.75</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="37">
@@ -11812,15 +13299,15 @@
       </c>
       <c r="H18" s="38">
         <f t="shared" si="4"/>
-        <v>0.15092771232944333</v>
+        <v>0.24634000000000003</v>
       </c>
       <c r="I18" s="39">
         <f t="shared" si="0"/>
-        <v>0.16678881840606721</v>
+        <v>0.25798500000000002</v>
       </c>
       <c r="J18" s="40">
         <f t="shared" si="0"/>
-        <v>0.17481937144437917</v>
+        <v>0.26975000000000005</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11829,15 +13316,15 @@
       </c>
       <c r="C19" s="6">
         <f t="shared" si="1"/>
-        <v>0.58137767414994534</v>
+        <v>0.84</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="2"/>
-        <v>0.62609903369994113</v>
+        <v>0.87</v>
       </c>
       <c r="E19" s="11">
         <f t="shared" si="3"/>
-        <v>0.64845971347493903</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="41">
@@ -11845,15 +13332,15 @@
       </c>
       <c r="H19" s="34">
         <f t="shared" si="4"/>
-        <v>0.19272125479533203</v>
+        <v>0.31309759999999998</v>
       </c>
       <c r="I19" s="35">
         <f t="shared" si="0"/>
-        <v>0.21261858208728063</v>
+        <v>0.32789239999999997</v>
       </c>
       <c r="J19" s="36">
         <f t="shared" si="0"/>
-        <v>0.22271124573325493</v>
+        <v>0.34285999999999994</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11862,15 +13349,15 @@
       </c>
       <c r="C20" s="6">
         <f t="shared" si="1"/>
-        <v>0.67827395317493633</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" si="2"/>
-        <v>0.73044887264993141</v>
+        <v>1.0150000000000001</v>
       </c>
       <c r="E20" s="11">
         <f t="shared" si="3"/>
-        <v>0.7565363323874289</v>
+        <v>1.05</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="37">
@@ -11878,15 +13365,15 @@
       </c>
       <c r="H20" s="38">
         <f t="shared" si="4"/>
-        <v>0.23631746392788741</v>
+        <v>0.38361840000000003</v>
       </c>
       <c r="I20" s="39">
         <f t="shared" si="0"/>
-        <v>0.26053901243516076</v>
+        <v>0.4018366000000001</v>
       </c>
       <c r="J20" s="40">
         <f t="shared" si="0"/>
-        <v>0.27284578668879744</v>
+        <v>0.42029000000000005</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11895,15 +13382,15 @@
       </c>
       <c r="C21" s="6">
         <f t="shared" si="1"/>
-        <v>0.77517023219992709</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" si="2"/>
-        <v>0.83479871159992158</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="E21" s="11">
         <f t="shared" si="3"/>
-        <v>0.86461295129991866</v>
+        <v>1.2</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="41">
@@ -11911,15 +13398,15 @@
       </c>
       <c r="H21" s="34">
         <f t="shared" si="4"/>
-        <v>0.2817163397271093</v>
+        <v>0.45790240000000004</v>
       </c>
       <c r="I21" s="35">
         <f t="shared" si="0"/>
-        <v>0.31055010944970751</v>
+        <v>0.47981759999999996</v>
       </c>
       <c r="J21" s="36">
         <f t="shared" si="0"/>
-        <v>0.32522299431100665</v>
+        <v>0.50203999999999993</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11928,15 +13415,15 @@
       </c>
       <c r="C22" s="6">
         <f t="shared" si="1"/>
-        <v>0.87206651122491796</v>
+        <v>1.26</v>
       </c>
       <c r="D22" s="6">
         <f t="shared" si="2"/>
-        <v>0.93914855054991164</v>
+        <v>1.3049999999999999</v>
       </c>
       <c r="E22" s="11">
         <f t="shared" si="3"/>
-        <v>0.97268957021240843</v>
+        <v>1.3499999999999999</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="37">
@@ -11944,15 +13431,15 @@
       </c>
       <c r="H22" s="38">
         <f t="shared" si="4"/>
-        <v>0.328917882192998</v>
+        <v>0.53594960000000003</v>
       </c>
       <c r="I22" s="39">
         <f t="shared" si="0"/>
-        <v>0.36265187313092095</v>
+        <v>0.56183539999999998</v>
       </c>
       <c r="J22" s="40">
         <f t="shared" si="0"/>
-        <v>0.37984286859988237</v>
+        <v>0.58810999999999991</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11961,15 +13448,15 @@
       </c>
       <c r="C23" s="6">
         <f t="shared" si="1"/>
-        <v>0.96896279024990883</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="2"/>
-        <v>1.0434983894999019</v>
+        <v>1.4500000000000002</v>
       </c>
       <c r="E23" s="11">
         <f t="shared" si="3"/>
-        <v>1.0807661891248985</v>
+        <v>1.5</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="41">
@@ -11977,15 +13464,15 @@
       </c>
       <c r="H23" s="34">
         <f t="shared" si="4"/>
-        <v>0.37792209132555332</v>
+        <v>0.61776000000000009</v>
       </c>
       <c r="I23" s="35">
         <f t="shared" si="0"/>
-        <v>0.41684430347880108</v>
+        <v>0.64789000000000008</v>
       </c>
       <c r="J23" s="36">
         <f t="shared" si="0"/>
-        <v>0.43670540955542503</v>
+        <v>0.67849999999999999</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11994,15 +13481,15 @@
       </c>
       <c r="C24" s="6">
         <f t="shared" si="1"/>
-        <v>1.0658590692748997</v>
+        <v>1.54</v>
       </c>
       <c r="D24" s="6">
         <f t="shared" si="2"/>
-        <v>1.1478482284498921</v>
+        <v>1.595</v>
       </c>
       <c r="E24" s="11">
         <f t="shared" si="3"/>
-        <v>1.1888428080373881</v>
+        <v>1.65</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="37">
@@ -12010,15 +13497,15 @@
       </c>
       <c r="H24" s="38">
         <f t="shared" si="4"/>
-        <v>0.42872896712477526</v>
+        <v>0.7033336</v>
       </c>
       <c r="I24" s="39">
         <f t="shared" si="0"/>
-        <v>0.47312740049334778</v>
+        <v>0.7379813999999999</v>
       </c>
       <c r="J24" s="40">
         <f t="shared" si="0"/>
-        <v>0.49581061717763397</v>
+        <v>0.77320999999999984</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12027,15 +13514,15 @@
       </c>
       <c r="C25" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627553482998907</v>
+        <v>1.68</v>
       </c>
       <c r="D25" s="6">
         <f t="shared" si="2"/>
-        <v>1.2521980673998823</v>
+        <v>1.74</v>
       </c>
       <c r="E25" s="11">
         <f t="shared" si="3"/>
-        <v>1.2969194269498781</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="41">
@@ -12043,15 +13530,15 @@
       </c>
       <c r="H25" s="34">
         <f t="shared" si="4"/>
-        <v>0.48133850959066404</v>
+        <v>0.79267039999999989</v>
       </c>
       <c r="I25" s="35">
         <f t="shared" si="0"/>
-        <v>0.53150116417456117</v>
+        <v>0.8321096</v>
       </c>
       <c r="J25" s="36">
         <f t="shared" si="0"/>
-        <v>0.55715849146650986</v>
+        <v>0.87223999999999979</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12060,15 +13547,15 @@
       </c>
       <c r="C26" s="6">
         <f t="shared" si="1"/>
-        <v>1.2596516273248815</v>
+        <v>1.82</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" si="2"/>
-        <v>1.3565479063498724</v>
+        <v>1.885</v>
       </c>
       <c r="E26" s="11">
         <f t="shared" si="3"/>
-        <v>1.4049960458623678</v>
+        <v>1.9500000000000002</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="37">
@@ -12076,15 +13563,15 @@
       </c>
       <c r="H26" s="38">
         <f t="shared" si="4"/>
-        <v>0.53575071872321922</v>
+        <v>0.88577040000000007</v>
       </c>
       <c r="I26" s="39">
         <f t="shared" si="0"/>
-        <v>0.59196559452244135</v>
+        <v>0.93027460000000006</v>
       </c>
       <c r="J26" s="40">
         <f t="shared" si="0"/>
-        <v>0.62074903242205237</v>
+        <v>0.97559000000000007</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12093,15 +13580,15 @@
       </c>
       <c r="C27" s="6">
         <f t="shared" si="1"/>
-        <v>1.3565479063498727</v>
+        <v>1.9600000000000002</v>
       </c>
       <c r="D27" s="6">
         <f t="shared" si="2"/>
-        <v>1.4608977452998628</v>
+        <v>2.0300000000000002</v>
       </c>
       <c r="E27" s="11">
         <f t="shared" si="3"/>
-        <v>1.5130726647748578</v>
+        <v>2.1</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="41">
@@ -12109,15 +13596,15 @@
       </c>
       <c r="H27" s="34">
         <f t="shared" si="4"/>
-        <v>0.59196559452244146</v>
+        <v>0.98263360000000011</v>
       </c>
       <c r="I27" s="35">
         <f t="shared" si="0"/>
-        <v>0.65452069153698822</v>
+        <v>1.0324764000000002</v>
       </c>
       <c r="J27" s="36">
         <f t="shared" si="0"/>
-        <v>0.6865822400442616</v>
+        <v>1.0832600000000001</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12126,15 +13613,15 @@
       </c>
       <c r="C28" s="6">
         <f t="shared" si="1"/>
-        <v>1.4534441853748632</v>
+        <v>2.1</v>
       </c>
       <c r="D28" s="6">
         <f t="shared" si="2"/>
-        <v>1.5652475842498528</v>
+        <v>2.1749999999999998</v>
       </c>
       <c r="E28" s="11">
         <f t="shared" si="3"/>
-        <v>1.6211492836873473</v>
+        <v>2.25</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="37">
@@ -12142,15 +13629,15 @@
       </c>
       <c r="H28" s="38">
         <f t="shared" si="4"/>
-        <v>0.64998313698832999</v>
+        <v>1.0832600000000001</v>
       </c>
       <c r="I28" s="39">
         <f t="shared" si="0"/>
-        <v>0.71916645521820166</v>
+        <v>1.1387149999999999</v>
       </c>
       <c r="J28" s="40">
         <f t="shared" si="0"/>
-        <v>0.75465811433313723</v>
+        <v>1.1952500000000001</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12159,15 +13646,15 @@
       </c>
       <c r="C29" s="6">
         <f t="shared" si="1"/>
-        <v>1.5503404643998542</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="D29" s="6">
         <f t="shared" si="2"/>
-        <v>1.6695974231998432</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="E29" s="11">
         <f t="shared" si="3"/>
-        <v>1.7292259025998373</v>
+        <v>2.4</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="41">
@@ -12175,15 +13662,15 @@
       </c>
       <c r="H29" s="34">
         <f t="shared" si="4"/>
-        <v>0.70980334612088536</v>
+        <v>1.1876496000000003</v>
       </c>
       <c r="I29" s="35">
         <f t="shared" si="0"/>
-        <v>0.78590288556608179</v>
+        <v>1.2489904000000001</v>
       </c>
       <c r="J29" s="36">
         <f t="shared" si="0"/>
-        <v>0.82497665528867981</v>
+        <v>1.3115600000000001</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12192,15 +13679,15 @@
       </c>
       <c r="C30" s="6">
         <f t="shared" si="1"/>
-        <v>1.6472367434248449</v>
+        <v>2.3800000000000003</v>
       </c>
       <c r="D30" s="6">
         <f t="shared" si="2"/>
-        <v>1.7739472621498333</v>
+        <v>2.4650000000000003</v>
       </c>
       <c r="E30" s="11">
         <f t="shared" si="3"/>
-        <v>1.8373025215123273</v>
+        <v>2.5500000000000003</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="37">
@@ -12208,15 +13695,15 @@
       </c>
       <c r="H30" s="38">
         <f t="shared" si="4"/>
-        <v>0.77142622192010724</v>
+        <v>1.2958024000000004</v>
       </c>
       <c r="I30" s="39">
         <f t="shared" si="0"/>
-        <v>0.8547299825806286</v>
+        <v>1.3633026000000006</v>
       </c>
       <c r="J30" s="40">
         <f t="shared" si="0"/>
-        <v>0.89753786291088911</v>
+        <v>1.4321900000000003</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12225,15 +13712,15 @@
       </c>
       <c r="C31" s="6">
         <f t="shared" si="1"/>
-        <v>1.7441330224498359</v>
+        <v>2.52</v>
       </c>
       <c r="D31" s="6">
         <f t="shared" si="2"/>
-        <v>1.8782971010998233</v>
+        <v>2.61</v>
       </c>
       <c r="E31" s="11">
         <f t="shared" si="3"/>
-        <v>1.9453791404248169</v>
+        <v>2.6999999999999997</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="41">
@@ -12241,15 +13728,15 @@
       </c>
       <c r="H31" s="34">
         <f t="shared" si="4"/>
-        <v>0.83485176438599595</v>
+        <v>1.4077184</v>
       </c>
       <c r="I31" s="35">
         <f t="shared" si="4"/>
-        <v>0.92564774626184188</v>
+        <v>1.4816516</v>
       </c>
       <c r="J31" s="36">
         <f t="shared" si="4"/>
-        <v>0.97234173719976458</v>
+        <v>1.5571399999999997</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12258,15 +13745,15 @@
       </c>
       <c r="C32" s="6">
         <f t="shared" si="1"/>
-        <v>1.8410293014748269</v>
+        <v>2.66</v>
       </c>
       <c r="D32" s="6">
         <f t="shared" si="2"/>
-        <v>1.9826469400498137</v>
+        <v>2.7549999999999999</v>
       </c>
       <c r="E32" s="11">
         <f t="shared" si="3"/>
-        <v>2.0534557593373068</v>
+        <v>2.85</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="37">
@@ -12274,15 +13761,15 @@
       </c>
       <c r="H32" s="38">
         <f t="shared" si="4"/>
-        <v>0.90007997351855151</v>
+        <v>1.5233976000000002</v>
       </c>
       <c r="I32" s="39">
         <f t="shared" si="4"/>
-        <v>0.99865617660972206</v>
+        <v>1.6040373999999999</v>
       </c>
       <c r="J32" s="40">
         <f t="shared" si="4"/>
-        <v>1.0493882781553074</v>
+        <v>1.6864100000000002</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12291,15 +13778,15 @@
       </c>
       <c r="C33" s="6">
         <f t="shared" si="1"/>
-        <v>1.9379255804998177</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="D33" s="6">
         <f t="shared" si="2"/>
-        <v>2.0869967789998038</v>
+        <v>2.9000000000000004</v>
       </c>
       <c r="E33" s="11">
         <f t="shared" si="3"/>
-        <v>2.161532378249797</v>
+        <v>3</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="41">
@@ -12307,15 +13794,15 @@
       </c>
       <c r="H33" s="34">
         <f t="shared" si="4"/>
-        <v>0.96711084931777325</v>
+        <v>1.6428400000000003</v>
       </c>
       <c r="I33" s="35">
         <f t="shared" si="4"/>
-        <v>1.073755273624269</v>
+        <v>1.7304600000000006</v>
       </c>
       <c r="J33" s="36">
         <f t="shared" si="4"/>
-        <v>1.1286774857775168</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12324,15 +13811,15 @@
       </c>
       <c r="C34" s="6">
         <f t="shared" si="1"/>
-        <v>2.0348218595248087</v>
+        <v>2.94</v>
       </c>
       <c r="D34" s="6">
         <f t="shared" si="2"/>
-        <v>2.1913466179497938</v>
+        <v>3.0449999999999999</v>
       </c>
       <c r="E34" s="11">
         <f t="shared" si="3"/>
-        <v>2.2696089971622864</v>
+        <v>3.15</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="37">
@@ -12340,15 +13827,15 @@
       </c>
       <c r="H34" s="38">
         <f t="shared" si="4"/>
-        <v>1.0359443917836624</v>
+        <v>1.7660456</v>
       </c>
       <c r="I34" s="39">
         <f t="shared" si="4"/>
-        <v>1.1509450373054821</v>
+        <v>1.8609194</v>
       </c>
       <c r="J34" s="40">
         <f t="shared" si="4"/>
-        <v>1.2102093600663923</v>
+        <v>1.9579100000000003</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12357,15 +13844,15 @@
       </c>
       <c r="C35" s="6">
         <f t="shared" si="1"/>
-        <v>2.1317181385497994</v>
+        <v>3.08</v>
       </c>
       <c r="D35" s="6">
         <f t="shared" si="2"/>
-        <v>2.2956964568997842</v>
+        <v>3.19</v>
       </c>
       <c r="E35" s="11">
         <f t="shared" si="3"/>
-        <v>2.3776856160747761</v>
+        <v>3.3</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="41">
@@ -12373,15 +13860,15 @@
       </c>
       <c r="H35" s="34">
         <f t="shared" si="4"/>
-        <v>1.1065806009162173</v>
+        <v>1.8930144</v>
       </c>
       <c r="I35" s="35">
         <f t="shared" si="4"/>
-        <v>1.2302254676533624</v>
+        <v>1.9954156000000001</v>
       </c>
       <c r="J35" s="36">
         <f t="shared" si="4"/>
-        <v>1.2939839010219345</v>
+        <v>2.1001399999999997</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12390,15 +13877,15 @@
       </c>
       <c r="C36" s="6">
         <f t="shared" si="1"/>
-        <v>2.2286144175747906</v>
+        <v>3.22</v>
       </c>
       <c r="D36" s="6">
         <f t="shared" si="2"/>
-        <v>2.4000462958497746</v>
+        <v>3.335</v>
       </c>
       <c r="E36" s="11">
         <f t="shared" si="3"/>
-        <v>2.4857622349872663</v>
+        <v>3.45</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="37">
@@ -12406,15 +13893,15 @@
       </c>
       <c r="H36" s="38">
         <f t="shared" si="4"/>
-        <v>1.1790194767154396</v>
+        <v>2.0237464000000003</v>
       </c>
       <c r="I36" s="39">
         <f t="shared" si="4"/>
-        <v>1.3115965646679093</v>
+        <v>2.1339485999999996</v>
       </c>
       <c r="J36" s="40">
         <f t="shared" si="4"/>
-        <v>1.3800011086441442</v>
+        <v>2.2466900000000001</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12423,15 +13910,15 @@
       </c>
       <c r="C37" s="6">
         <f t="shared" si="1"/>
-        <v>2.3255106965997814</v>
+        <v>3.36</v>
       </c>
       <c r="D37" s="6">
         <f t="shared" si="2"/>
-        <v>2.5043961347997645</v>
+        <v>3.48</v>
       </c>
       <c r="E37" s="11">
         <f t="shared" si="3"/>
-        <v>2.5938388538997561</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="41">
@@ -12439,15 +13926,15 @@
       </c>
       <c r="H37" s="34">
         <f t="shared" si="4"/>
-        <v>1.2532610191813283</v>
+        <v>2.1582415999999998</v>
       </c>
       <c r="I37" s="35">
         <f t="shared" si="4"/>
-        <v>1.3950583283491225</v>
+        <v>2.2765184000000001</v>
       </c>
       <c r="J37" s="36">
         <f t="shared" si="4"/>
-        <v>1.46826098293302</v>
+        <v>2.3975599999999995</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12456,15 +13943,15 @@
       </c>
       <c r="C38" s="6">
         <f t="shared" si="1"/>
-        <v>2.4224069756247721</v>
+        <v>3.5</v>
       </c>
       <c r="D38" s="6">
         <f t="shared" si="2"/>
-        <v>2.6087459737497545</v>
+        <v>3.625</v>
       </c>
       <c r="E38" s="11">
         <f t="shared" si="3"/>
-        <v>2.7019154728122459</v>
+        <v>3.75</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="37">
@@ -12472,15 +13959,15 @@
       </c>
       <c r="H38" s="38">
         <f t="shared" si="4"/>
-        <v>1.3293052283138835</v>
+        <v>2.2964999999999995</v>
       </c>
       <c r="I38" s="39">
         <f t="shared" si="4"/>
-        <v>1.4806107586970025</v>
+        <v>2.4231250000000002</v>
       </c>
       <c r="J38" s="40">
         <f t="shared" si="4"/>
-        <v>1.5587635238885624</v>
+        <v>2.5527500000000001</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12489,15 +13976,15 @@
       </c>
       <c r="C39" s="6">
         <f t="shared" si="1"/>
-        <v>2.5193032546497629</v>
+        <v>3.64</v>
       </c>
       <c r="D39" s="6">
         <f t="shared" si="2"/>
-        <v>2.7130958126997449</v>
+        <v>3.77</v>
       </c>
       <c r="E39" s="11">
         <f t="shared" si="3"/>
-        <v>2.8099920917247356</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="41">
@@ -12505,15 +13992,15 @@
       </c>
       <c r="H39" s="34">
         <f t="shared" si="4"/>
-        <v>1.4071521041131054</v>
+        <v>2.4385216000000001</v>
       </c>
       <c r="I39" s="35">
         <f t="shared" si="4"/>
-        <v>1.5682538557115495</v>
+        <v>2.5737684000000001</v>
       </c>
       <c r="J39" s="36">
         <f t="shared" si="4"/>
-        <v>1.6515087315107715</v>
+        <v>2.7122600000000001</v>
       </c>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12522,15 +14009,15 @@
       </c>
       <c r="C40" s="6">
         <f t="shared" si="1"/>
-        <v>2.6161995336747541</v>
+        <v>3.7800000000000002</v>
       </c>
       <c r="D40" s="6">
         <f t="shared" si="2"/>
-        <v>2.8174456516497353</v>
+        <v>3.915</v>
       </c>
       <c r="E40" s="11">
         <f t="shared" si="3"/>
-        <v>2.9180687106372254</v>
+        <v>4.0500000000000007</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="37">
@@ -12538,15 +14025,15 @@
       </c>
       <c r="H40" s="38">
         <f t="shared" si="4"/>
-        <v>1.4868016465789944</v>
+        <v>2.5843064000000004</v>
       </c>
       <c r="I40" s="39">
         <f t="shared" si="4"/>
-        <v>1.6579876193927632</v>
+        <v>2.7284485999999997</v>
       </c>
       <c r="J40" s="40">
         <f t="shared" si="4"/>
-        <v>1.7464966057996472</v>
+        <v>2.8760900000000009</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12555,15 +14042,15 @@
       </c>
       <c r="C41" s="6">
         <f t="shared" si="1"/>
-        <v>2.7130958126997453</v>
+        <v>3.9200000000000004</v>
       </c>
       <c r="D41" s="6">
         <f t="shared" si="2"/>
-        <v>2.9217954905997257</v>
+        <v>4.0600000000000005</v>
       </c>
       <c r="E41" s="11">
         <f t="shared" si="3"/>
-        <v>3.0261453295497156</v>
+        <v>4.2</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="41">
@@ -12571,15 +14058,15 @@
       </c>
       <c r="H41" s="34">
         <f t="shared" si="4"/>
-        <v>1.5682538557115497</v>
+        <v>2.7338544000000002</v>
       </c>
       <c r="I41" s="35">
         <f t="shared" si="4"/>
-        <v>1.7498120497406433</v>
+        <v>2.8871656000000003</v>
       </c>
       <c r="J41" s="36">
         <f t="shared" si="4"/>
-        <v>1.8437271467551901</v>
+        <v>3.0442399999999998</v>
       </c>
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12588,15 +14075,15 @@
       </c>
       <c r="C42" s="6">
         <f t="shared" si="1"/>
-        <v>2.8099920917247352</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="D42" s="6">
         <f t="shared" si="2"/>
-        <v>3.0261453295497152</v>
+        <v>4.2050000000000001</v>
       </c>
       <c r="E42" s="11">
         <f t="shared" si="3"/>
-        <v>3.1342219484622054</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="37">
@@ -12604,15 +14091,15 @@
       </c>
       <c r="H42" s="38">
         <f t="shared" si="4"/>
-        <v>1.651508731510771</v>
+        <v>2.8871655999999994</v>
       </c>
       <c r="I42" s="39">
         <f t="shared" si="4"/>
-        <v>1.8437271467551897</v>
+        <v>3.0499193999999998</v>
       </c>
       <c r="J42" s="40">
         <f t="shared" si="4"/>
-        <v>1.943200354377399</v>
+        <v>3.2167099999999995</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12621,15 +14108,15 @@
       </c>
       <c r="C43" s="6">
         <f t="shared" si="1"/>
-        <v>2.9068883707497264</v>
+        <v>4.2</v>
       </c>
       <c r="D43" s="6">
         <f t="shared" si="2"/>
-        <v>3.1304951684997055</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="E43" s="11">
         <f t="shared" si="3"/>
-        <v>3.2422985673746947</v>
+        <v>4.5</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="41">
@@ -12637,15 +14124,15 @@
       </c>
       <c r="H43" s="34">
         <f t="shared" si="4"/>
-        <v>1.7365662739766601</v>
+        <v>3.0442399999999998</v>
       </c>
       <c r="I43" s="35">
         <f t="shared" si="4"/>
-        <v>1.9397329104364034</v>
+        <v>3.2167099999999995</v>
       </c>
       <c r="J43" s="36">
         <f t="shared" si="4"/>
-        <v>2.0449162286662745</v>
+        <v>3.3935</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12654,15 +14141,15 @@
       </c>
       <c r="C44" s="6">
         <f t="shared" si="1"/>
-        <v>3.0037846497747176</v>
+        <v>4.34</v>
       </c>
       <c r="D44" s="6">
         <f t="shared" si="2"/>
-        <v>3.2348450074496955</v>
+        <v>4.4950000000000001</v>
       </c>
       <c r="E44" s="11">
         <f t="shared" si="3"/>
-        <v>3.3503751862871849</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="37">
@@ -12670,15 +14157,15 @@
       </c>
       <c r="H44" s="38">
         <f t="shared" si="4"/>
-        <v>1.8234264831092155</v>
+        <v>3.2050775999999996</v>
       </c>
       <c r="I44" s="39">
         <f t="shared" si="4"/>
-        <v>2.0378293407842829</v>
+        <v>3.3875374000000003</v>
       </c>
       <c r="J44" s="40">
         <f t="shared" si="4"/>
-        <v>2.1488747696218171</v>
+        <v>3.5746100000000003</v>
       </c>
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12687,15 +14174,15 @@
       </c>
       <c r="C45" s="6">
         <f t="shared" si="1"/>
-        <v>3.1006809287997084</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="D45" s="6">
         <f t="shared" si="2"/>
-        <v>3.3391948463996863</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="E45" s="11">
         <f t="shared" si="3"/>
-        <v>3.4584518051996747</v>
+        <v>4.8</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="41">
@@ -12703,15 +14190,15 @@
       </c>
       <c r="H45" s="34">
         <f t="shared" si="4"/>
-        <v>1.9120893589084376</v>
+        <v>3.3696784000000002</v>
       </c>
       <c r="I45" s="35">
         <f t="shared" si="4"/>
-        <v>2.13801643779883</v>
+        <v>3.5624015999999998</v>
       </c>
       <c r="J45" s="36">
         <f t="shared" si="4"/>
-        <v>2.2550759772440263</v>
+        <v>3.7600399999999996</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12720,15 +14207,15 @@
       </c>
       <c r="C46" s="6">
         <f t="shared" si="1"/>
-        <v>3.1975772078246991</v>
+        <v>4.62</v>
       </c>
       <c r="D46" s="6">
         <f t="shared" si="2"/>
-        <v>3.4435446853496763</v>
+        <v>4.7850000000000001</v>
       </c>
       <c r="E46" s="11">
         <f t="shared" si="3"/>
-        <v>3.5665284241121644</v>
+        <v>4.95</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="37">
@@ -12736,15 +14223,15 @@
       </c>
       <c r="H46" s="38">
         <f t="shared" si="4"/>
-        <v>2.0025549013743258</v>
+        <v>3.5380423999999997</v>
       </c>
       <c r="I46" s="39">
         <f t="shared" si="4"/>
-        <v>2.2402942014800433</v>
+        <v>3.7413026</v>
       </c>
       <c r="J46" s="40">
         <f t="shared" si="4"/>
-        <v>2.3635198515329017</v>
+        <v>3.9497900000000001</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12753,15 +14240,15 @@
       </c>
       <c r="C47" s="6">
         <f t="shared" si="1"/>
-        <v>3.2944734868496899</v>
+        <v>4.7600000000000007</v>
       </c>
       <c r="D47" s="6">
         <f t="shared" si="2"/>
-        <v>3.5478945242996667</v>
+        <v>4.9300000000000006</v>
       </c>
       <c r="E47" s="11">
         <f t="shared" si="3"/>
-        <v>3.6746050430246546</v>
+        <v>5.1000000000000005</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="41">
@@ -12769,15 +14256,15 @@
       </c>
       <c r="H47" s="34">
         <f t="shared" si="4"/>
-        <v>2.0948231105068813</v>
+        <v>3.7101696000000008</v>
       </c>
       <c r="I47" s="35">
         <f t="shared" si="4"/>
-        <v>2.3446626318279242</v>
+        <v>3.9242404000000009</v>
       </c>
       <c r="J47" s="36">
         <f t="shared" si="4"/>
-        <v>2.4742063924884445</v>
+        <v>4.143860000000001</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12786,15 +14273,15 @@
       </c>
       <c r="C48" s="6">
         <f t="shared" si="1"/>
-        <v>3.3913697658746806</v>
+        <v>4.8999999999999995</v>
       </c>
       <c r="D48" s="6">
         <f t="shared" si="2"/>
-        <v>3.6522443632496562</v>
+        <v>5.0749999999999993</v>
       </c>
       <c r="E48" s="11">
         <f t="shared" si="3"/>
-        <v>3.7826816619371435</v>
+        <v>5.25</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="37">
@@ -12802,15 +14289,15 @@
       </c>
       <c r="H48" s="38">
         <f t="shared" si="4"/>
-        <v>2.1888939863061032</v>
+        <v>3.8860599999999992</v>
       </c>
       <c r="I48" s="39">
         <f t="shared" si="4"/>
-        <v>2.45112172884247</v>
+        <v>4.1112149999999987</v>
       </c>
       <c r="J48" s="40">
         <f t="shared" si="4"/>
-        <v>2.5871356001106531</v>
+        <v>4.3422500000000008</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12819,15 +14306,15 @@
       </c>
       <c r="C49" s="6">
         <f t="shared" si="1"/>
-        <v>3.4882660448996718</v>
+        <v>5.04</v>
       </c>
       <c r="D49" s="6">
         <f t="shared" si="2"/>
-        <v>3.7565942021996466</v>
+        <v>5.22</v>
       </c>
       <c r="E49" s="11">
         <f t="shared" si="3"/>
-        <v>3.8907582808496337</v>
+        <v>5.3999999999999995</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="41">
@@ -12835,15 +14322,15 @@
       </c>
       <c r="H49" s="34">
         <f t="shared" si="4"/>
-        <v>2.284767528771992</v>
+        <v>4.0657136000000005</v>
       </c>
       <c r="I49" s="35">
         <f t="shared" si="4"/>
-        <v>2.5596714925236834</v>
+        <v>4.3022263999999995</v>
       </c>
       <c r="J49" s="36">
         <f t="shared" si="4"/>
-        <v>2.7023074743995292</v>
+        <v>4.5449599999999997</v>
       </c>
     </row>
     <row r="50" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12852,30 +14339,30 @@
       </c>
       <c r="C50" s="6">
         <f t="shared" si="1"/>
-        <v>3.5851623239246626</v>
+        <v>5.18</v>
       </c>
       <c r="D50" s="6">
         <f t="shared" si="2"/>
-        <v>3.8609440411496365</v>
+        <v>5.3650000000000002</v>
       </c>
       <c r="E50" s="11">
         <f t="shared" si="3"/>
-        <v>3.9988348997621239</v>
+        <v>5.55</v>
       </c>
       <c r="G50" s="37">
         <v>0.37</v>
       </c>
       <c r="H50" s="38">
         <f t="shared" si="4"/>
-        <v>2.3824437379045471</v>
+        <v>4.2491304000000003</v>
       </c>
       <c r="I50" s="39">
         <f t="shared" si="4"/>
-        <v>2.6703119228715635</v>
+        <v>4.4972746000000008</v>
       </c>
       <c r="J50" s="40">
         <f t="shared" si="4"/>
-        <v>2.8197220153550719</v>
+        <v>4.7519900000000002</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12884,30 +14371,30 @@
       </c>
       <c r="C51" s="6">
         <f t="shared" si="1"/>
-        <v>3.6820586029496538</v>
+        <v>5.32</v>
       </c>
       <c r="D51" s="6">
         <f t="shared" si="2"/>
-        <v>3.9652938800996274</v>
+        <v>5.51</v>
       </c>
       <c r="E51" s="11">
         <f t="shared" si="3"/>
-        <v>4.1069115186746137</v>
+        <v>5.7</v>
       </c>
       <c r="G51" s="41">
         <v>0.38</v>
       </c>
       <c r="H51" s="34">
         <f t="shared" si="4"/>
-        <v>2.4819226137037695</v>
+        <v>4.4363104000000009</v>
       </c>
       <c r="I51" s="35">
         <f t="shared" si="4"/>
-        <v>2.7830430198861111</v>
+        <v>4.6963596000000001</v>
       </c>
       <c r="J51" s="36">
         <f t="shared" si="4"/>
-        <v>2.9393792229772813</v>
+        <v>4.9633400000000005</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12916,30 +14403,30 @@
       </c>
       <c r="C52" s="6">
         <f t="shared" si="1"/>
-        <v>3.7789548819746446</v>
+        <v>5.46</v>
       </c>
       <c r="D52" s="6">
         <f t="shared" si="2"/>
-        <v>4.0696437190496173</v>
+        <v>5.6550000000000002</v>
       </c>
       <c r="E52" s="11">
         <f t="shared" si="3"/>
-        <v>4.2149881375871034</v>
+        <v>5.8500000000000005</v>
       </c>
       <c r="G52" s="42">
         <v>0.39</v>
       </c>
       <c r="H52" s="38">
         <f t="shared" si="4"/>
-        <v>2.5832041561696579</v>
+        <v>4.6272536000000004</v>
       </c>
       <c r="I52" s="39">
         <f t="shared" si="4"/>
-        <v>2.8978647835673246</v>
+        <v>4.8994814000000009</v>
       </c>
       <c r="J52" s="40">
         <f t="shared" si="4"/>
-        <v>3.0612790972661568</v>
+        <v>5.1790100000000008</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12948,30 +14435,30 @@
       </c>
       <c r="C53" s="10">
         <f t="shared" si="1"/>
-        <v>3.8758511609996353</v>
+        <v>5.6000000000000005</v>
       </c>
       <c r="D53" s="10">
         <f t="shared" si="2"/>
-        <v>4.1739935579996077</v>
+        <v>5.8000000000000007</v>
       </c>
       <c r="E53" s="12">
         <f t="shared" si="3"/>
-        <v>4.3230647564995941</v>
+        <v>6</v>
       </c>
       <c r="G53" s="43">
         <v>0.4</v>
       </c>
       <c r="H53" s="44">
         <f t="shared" si="4"/>
-        <v>2.6862883653022132</v>
+        <v>4.8219600000000016</v>
       </c>
       <c r="I53" s="45">
         <f t="shared" si="4"/>
-        <v>3.0147772139152047</v>
+        <v>5.1066400000000014</v>
       </c>
       <c r="J53" s="46">
         <f t="shared" si="4"/>
-        <v>3.1854216382217002</v>
+        <v>5.399</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12987,6 +14474,1485 @@
     <mergeCell ref="G13:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="86" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:J54"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.7109375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="13" customWidth="1"/>
+    <col min="9" max="10" width="12" style="13" customWidth="1"/>
+    <col min="11" max="32" width="8.7109375" style="14" customWidth="1"/>
+    <col min="33" max="16384" width="14.42578125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+    </row>
+    <row r="2" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="19">
+        <v>7</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="20"/>
+      <c r="C5" s="21">
+        <v>7.25</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="22"/>
+      <c r="C6" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="24">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="25"/>
+      <c r="C8" s="21">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="C9" s="21">
+        <v>-3.1E-2</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="27">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="51">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
+    </row>
+    <row r="13" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="61"/>
+    </row>
+    <row r="14" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="55"/>
+      <c r="C14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="30" t="str">
+        <f>+CONCATENATE("L = ",C4,"''")</f>
+        <v>L = 7''</v>
+      </c>
+      <c r="I14" s="31" t="str">
+        <f>+CONCATENATE("L = ",C5,"''")</f>
+        <v>L = 7.25''</v>
+      </c>
+      <c r="J14" s="32" t="str">
+        <f>+CONCATENATE("L = ",C6,"''")</f>
+        <v>L = 7.5''</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="C15" s="6">
+        <f>B15*$C$4/$C$10</f>
+        <v>0.25454545454545457</v>
+      </c>
+      <c r="D15" s="6">
+        <f>B15*$C$5/$C$10</f>
+        <v>0.26363636363636361</v>
+      </c>
+      <c r="E15" s="11">
+        <f>B15*$C$6/$C$10</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="H15" s="34">
+        <f>$C$7*C15^2+$C$8*C15+$C$9</f>
+        <v>5.8965619834710756E-2</v>
+      </c>
+      <c r="I15" s="35">
+        <f t="shared" ref="I15:J30" si="0">$C$7*D15^2+$C$8*D15+$C$9</f>
+        <v>6.2408760330578517E-2</v>
+      </c>
+      <c r="J15" s="36">
+        <f t="shared" si="0"/>
+        <v>6.5867768595041315E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" ref="C16:C53" si="1">B16*$C$4/$C$10</f>
+        <v>0.38181818181818178</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" ref="D16:D53" si="2">B16*$C$5/$C$10</f>
+        <v>0.39545454545454545</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" ref="E16:E53" si="3">B16*$C$6/$C$10</f>
+        <v>0.40909090909090901</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="37">
+        <v>0.03</v>
+      </c>
+      <c r="H16" s="38">
+        <f t="shared" ref="H16:J53" si="4">$C$7*C16^2+$C$8*C16+$C$9</f>
+        <v>0.10861355371900827</v>
+      </c>
+      <c r="I16" s="39">
+        <f t="shared" si="0"/>
+        <v>0.1141174380165289</v>
+      </c>
+      <c r="J16" s="40">
+        <f t="shared" si="0"/>
+        <v>0.11965702479338841</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="1"/>
+        <v>0.50909090909090915</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="2"/>
+        <v>0.52727272727272723</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="3"/>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="41">
+        <v>0.04</v>
+      </c>
+      <c r="H17" s="34">
+        <f t="shared" si="4"/>
+        <v>0.16137157024793392</v>
+      </c>
+      <c r="I17" s="35">
+        <f t="shared" si="0"/>
+        <v>0.16916231404958679</v>
+      </c>
+      <c r="J17" s="36">
+        <f t="shared" si="0"/>
+        <v>0.17701652892561984</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="1"/>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.65909090909090917</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="3"/>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="H18" s="38">
+        <f t="shared" si="4"/>
+        <v>0.21723966942148762</v>
+      </c>
+      <c r="I18" s="39">
+        <f t="shared" si="0"/>
+        <v>0.22754338842975211</v>
+      </c>
+      <c r="J18" s="40">
+        <f t="shared" si="0"/>
+        <v>0.23794628099173551</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="1"/>
+        <v>0.76363636363636356</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" si="2"/>
+        <v>0.79090909090909089</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" si="3"/>
+        <v>0.81818181818181801</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="41">
+        <v>0.06</v>
+      </c>
+      <c r="H19" s="34">
+        <f t="shared" si="4"/>
+        <v>0.27621785123966947</v>
+      </c>
+      <c r="I19" s="35">
+        <f t="shared" si="0"/>
+        <v>0.28926066115702476</v>
+      </c>
+      <c r="J19" s="36">
+        <f t="shared" si="0"/>
+        <v>0.30244628099173543</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="1"/>
+        <v>0.89090909090909087</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" si="2"/>
+        <v>0.92272727272727273</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="3"/>
+        <v>0.95454545454545447</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H20" s="38">
+        <f t="shared" si="4"/>
+        <v>0.33830611570247937</v>
+      </c>
+      <c r="I20" s="39">
+        <f t="shared" si="0"/>
+        <v>0.35431413223140495</v>
+      </c>
+      <c r="J20" s="40">
+        <f t="shared" si="0"/>
+        <v>0.37051652892561981</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="1"/>
+        <v>1.0181818181818183</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0545454545454545</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="3"/>
+        <v>1.0909090909090908</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="41">
+        <v>0.08</v>
+      </c>
+      <c r="H21" s="34">
+        <f t="shared" si="4"/>
+        <v>0.40350446280991736</v>
+      </c>
+      <c r="I21" s="35">
+        <f t="shared" si="0"/>
+        <v>0.42270380165289256</v>
+      </c>
+      <c r="J21" s="36">
+        <f t="shared" si="0"/>
+        <v>0.44215702479338836</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="1"/>
+        <v>1.1454545454545453</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1863636363636363</v>
+      </c>
+      <c r="E22" s="11">
+        <f t="shared" si="3"/>
+        <v>1.2272727272727271</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="37">
+        <v>0.09</v>
+      </c>
+      <c r="H22" s="38">
+        <f t="shared" si="4"/>
+        <v>0.47181289256198333</v>
+      </c>
+      <c r="I22" s="39">
+        <f t="shared" si="0"/>
+        <v>0.49442966942148758</v>
+      </c>
+      <c r="J22" s="40">
+        <f t="shared" si="0"/>
+        <v>0.51736776859504119</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2727272727272727</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3181818181818183</v>
+      </c>
+      <c r="E23" s="11">
+        <f t="shared" si="3"/>
+        <v>1.3636363636363635</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="41">
+        <v>0.1</v>
+      </c>
+      <c r="H23" s="34">
+        <f t="shared" si="4"/>
+        <v>0.54323140495867761</v>
+      </c>
+      <c r="I23" s="35">
+        <f t="shared" si="0"/>
+        <v>0.56949173553719012</v>
+      </c>
+      <c r="J23" s="36">
+        <f t="shared" si="0"/>
+        <v>0.59614876033057851</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="2"/>
+        <v>1.45</v>
+      </c>
+      <c r="E24" s="11">
+        <f t="shared" si="3"/>
+        <v>1.4999999999999998</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="37">
+        <v>0.11</v>
+      </c>
+      <c r="H24" s="38">
+        <f t="shared" si="4"/>
+        <v>0.61775999999999998</v>
+      </c>
+      <c r="I24" s="39">
+        <f t="shared" si="0"/>
+        <v>0.64788999999999997</v>
+      </c>
+      <c r="J24" s="40">
+        <f t="shared" si="0"/>
+        <v>0.67849999999999977</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="1"/>
+        <v>1.5272727272727271</v>
+      </c>
+      <c r="D25" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5818181818181818</v>
+      </c>
+      <c r="E25" s="11">
+        <f t="shared" si="3"/>
+        <v>1.636363636363636</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="41">
+        <v>0.12</v>
+      </c>
+      <c r="H25" s="34">
+        <f t="shared" si="4"/>
+        <v>0.69539867768595032</v>
+      </c>
+      <c r="I25" s="35">
+        <f t="shared" si="0"/>
+        <v>0.72962446280991733</v>
+      </c>
+      <c r="J25" s="36">
+        <f t="shared" si="0"/>
+        <v>0.76442148760330564</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="8">
+        <v>0.13</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6545454545454545</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" si="2"/>
+        <v>1.7136363636363634</v>
+      </c>
+      <c r="E26" s="11">
+        <f t="shared" si="3"/>
+        <v>1.7727272727272727</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="37">
+        <v>0.13</v>
+      </c>
+      <c r="H26" s="38">
+        <f t="shared" si="4"/>
+        <v>0.77614743801652886</v>
+      </c>
+      <c r="I26" s="39">
+        <f t="shared" si="0"/>
+        <v>0.81469512396694199</v>
+      </c>
+      <c r="J26" s="40">
+        <f t="shared" si="0"/>
+        <v>0.85391322314049589</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="1"/>
+        <v>1.7818181818181817</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8454545454545455</v>
+      </c>
+      <c r="E27" s="11">
+        <f t="shared" si="3"/>
+        <v>1.9090909090909089</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="41">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H27" s="34">
+        <f t="shared" si="4"/>
+        <v>0.86000628099173559</v>
+      </c>
+      <c r="I27" s="35">
+        <f t="shared" si="0"/>
+        <v>0.9031019834710744</v>
+      </c>
+      <c r="J27" s="36">
+        <f t="shared" si="0"/>
+        <v>0.94697520661157009</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="1"/>
+        <v>1.9090909090909089</v>
+      </c>
+      <c r="D28" s="6">
+        <f t="shared" si="2"/>
+        <v>1.9772727272727268</v>
+      </c>
+      <c r="E28" s="11">
+        <f t="shared" si="3"/>
+        <v>2.0454545454545454</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="37">
+        <v>0.15</v>
+      </c>
+      <c r="H28" s="38">
+        <f t="shared" si="4"/>
+        <v>0.94697520661157009</v>
+      </c>
+      <c r="I28" s="39">
+        <f t="shared" si="0"/>
+        <v>0.99484504132231388</v>
+      </c>
+      <c r="J28" s="40">
+        <f t="shared" si="0"/>
+        <v>1.043607438016529</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="1"/>
+        <v>2.0363636363636366</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" si="2"/>
+        <v>2.1090909090909089</v>
+      </c>
+      <c r="E29" s="11">
+        <f t="shared" si="3"/>
+        <v>2.1818181818181817</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="41">
+        <v>0.16</v>
+      </c>
+      <c r="H29" s="34">
+        <f t="shared" si="4"/>
+        <v>1.0370542148760333</v>
+      </c>
+      <c r="I29" s="35">
+        <f t="shared" si="0"/>
+        <v>1.0899242975206611</v>
+      </c>
+      <c r="J29" s="36">
+        <f t="shared" si="0"/>
+        <v>1.143809917355372</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="1"/>
+        <v>2.1636363636363636</v>
+      </c>
+      <c r="D30" s="6">
+        <f t="shared" si="2"/>
+        <v>2.2409090909090912</v>
+      </c>
+      <c r="E30" s="11">
+        <f t="shared" si="3"/>
+        <v>2.3181818181818183</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="37">
+        <v>0.17</v>
+      </c>
+      <c r="H30" s="38">
+        <f t="shared" si="4"/>
+        <v>1.130243305785124</v>
+      </c>
+      <c r="I30" s="39">
+        <f t="shared" si="0"/>
+        <v>1.1883397520661161</v>
+      </c>
+      <c r="J30" s="40">
+        <f t="shared" si="0"/>
+        <v>1.2475826446280995</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="1"/>
+        <v>2.2909090909090906</v>
+      </c>
+      <c r="D31" s="6">
+        <f t="shared" si="2"/>
+        <v>2.3727272727272726</v>
+      </c>
+      <c r="E31" s="11">
+        <f t="shared" si="3"/>
+        <v>2.4545454545454541</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="41">
+        <v>0.18</v>
+      </c>
+      <c r="H31" s="34">
+        <f t="shared" si="4"/>
+        <v>1.2265424793388429</v>
+      </c>
+      <c r="I31" s="35">
+        <f t="shared" si="4"/>
+        <v>1.2900914049586778</v>
+      </c>
+      <c r="J31" s="36">
+        <f t="shared" si="4"/>
+        <v>1.3549256198347106</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="1"/>
+        <v>2.418181818181818</v>
+      </c>
+      <c r="D32" s="6">
+        <f t="shared" si="2"/>
+        <v>2.5045454545454544</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" si="3"/>
+        <v>2.5909090909090908</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="37">
+        <v>0.19</v>
+      </c>
+      <c r="H32" s="38">
+        <f t="shared" si="4"/>
+        <v>1.3259517355371899</v>
+      </c>
+      <c r="I32" s="39">
+        <f t="shared" si="4"/>
+        <v>1.3951792561983472</v>
+      </c>
+      <c r="J32" s="40">
+        <f t="shared" si="4"/>
+        <v>1.4658388429752065</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5454545454545454</v>
+      </c>
+      <c r="D33" s="6">
+        <f t="shared" si="2"/>
+        <v>2.6363636363636367</v>
+      </c>
+      <c r="E33" s="11">
+        <f t="shared" si="3"/>
+        <v>2.7272727272727271</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="H33" s="34">
+        <f t="shared" si="4"/>
+        <v>1.4284710743801654</v>
+      </c>
+      <c r="I33" s="35">
+        <f t="shared" si="4"/>
+        <v>1.5036033057851244</v>
+      </c>
+      <c r="J33" s="36">
+        <f t="shared" si="4"/>
+        <v>1.5803223140495868</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="1"/>
+        <v>2.6727272727272724</v>
+      </c>
+      <c r="D34" s="6">
+        <f t="shared" si="2"/>
+        <v>2.7681818181818181</v>
+      </c>
+      <c r="E34" s="11">
+        <f t="shared" si="3"/>
+        <v>2.8636363636363633</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="37">
+        <v>0.21</v>
+      </c>
+      <c r="H34" s="38">
+        <f t="shared" si="4"/>
+        <v>1.5341004958677684</v>
+      </c>
+      <c r="I34" s="39">
+        <f t="shared" si="4"/>
+        <v>1.6153635537190081</v>
+      </c>
+      <c r="J34" s="40">
+        <f t="shared" si="4"/>
+        <v>1.698376033057851</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="1"/>
+        <v>2.8</v>
+      </c>
+      <c r="D35" s="6">
+        <f t="shared" si="2"/>
+        <v>2.9</v>
+      </c>
+      <c r="E35" s="11">
+        <f t="shared" si="3"/>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="41">
+        <v>0.22</v>
+      </c>
+      <c r="H35" s="34">
+        <f t="shared" si="4"/>
+        <v>1.6428399999999999</v>
+      </c>
+      <c r="I35" s="35">
+        <f t="shared" si="4"/>
+        <v>1.7304600000000001</v>
+      </c>
+      <c r="J35" s="36">
+        <f t="shared" si="4"/>
+        <v>1.8199999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="1"/>
+        <v>2.9272727272727272</v>
+      </c>
+      <c r="D36" s="6">
+        <f t="shared" si="2"/>
+        <v>3.0318181818181817</v>
+      </c>
+      <c r="E36" s="11">
+        <f t="shared" si="3"/>
+        <v>3.1363636363636362</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="37">
+        <v>0.23</v>
+      </c>
+      <c r="H36" s="38">
+        <f t="shared" si="4"/>
+        <v>1.7546895867768597</v>
+      </c>
+      <c r="I36" s="39">
+        <f t="shared" si="4"/>
+        <v>1.8488926446280993</v>
+      </c>
+      <c r="J36" s="40">
+        <f t="shared" si="4"/>
+        <v>1.9451942148760333</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="1"/>
+        <v>3.0545454545454542</v>
+      </c>
+      <c r="D37" s="6">
+        <f t="shared" si="2"/>
+        <v>3.1636363636363636</v>
+      </c>
+      <c r="E37" s="11">
+        <f t="shared" si="3"/>
+        <v>3.272727272727272</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="41">
+        <v>0.24</v>
+      </c>
+      <c r="H37" s="34">
+        <f t="shared" si="4"/>
+        <v>1.8696492561983471</v>
+      </c>
+      <c r="I37" s="35">
+        <f t="shared" si="4"/>
+        <v>1.9706614876033057</v>
+      </c>
+      <c r="J37" s="36">
+        <f t="shared" si="4"/>
+        <v>2.0739586776859498</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C38" s="6">
+        <f t="shared" si="1"/>
+        <v>3.1818181818181817</v>
+      </c>
+      <c r="D38" s="6">
+        <f t="shared" si="2"/>
+        <v>3.295454545454545</v>
+      </c>
+      <c r="E38" s="11">
+        <f t="shared" si="3"/>
+        <v>3.4090909090909087</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="37">
+        <v>0.25</v>
+      </c>
+      <c r="H38" s="38">
+        <f t="shared" si="4"/>
+        <v>1.9877190082644629</v>
+      </c>
+      <c r="I38" s="39">
+        <f t="shared" si="4"/>
+        <v>2.0957665289256191</v>
+      </c>
+      <c r="J38" s="40">
+        <f t="shared" si="4"/>
+        <v>2.2062933884297515</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="C39" s="6">
+        <f t="shared" si="1"/>
+        <v>3.3090909090909091</v>
+      </c>
+      <c r="D39" s="6">
+        <f t="shared" si="2"/>
+        <v>3.4272727272727268</v>
+      </c>
+      <c r="E39" s="11">
+        <f t="shared" si="3"/>
+        <v>3.5454545454545454</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="41">
+        <v>0.26</v>
+      </c>
+      <c r="H39" s="34">
+        <f t="shared" si="4"/>
+        <v>2.1088988429752065</v>
+      </c>
+      <c r="I39" s="35">
+        <f t="shared" si="4"/>
+        <v>2.2242077685950408</v>
+      </c>
+      <c r="J39" s="36">
+        <f t="shared" si="4"/>
+        <v>2.3421983471074381</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="C40" s="6">
+        <f t="shared" si="1"/>
+        <v>3.4363636363636365</v>
+      </c>
+      <c r="D40" s="6">
+        <f t="shared" si="2"/>
+        <v>3.5590909090909086</v>
+      </c>
+      <c r="E40" s="11">
+        <f t="shared" si="3"/>
+        <v>3.6818181818181821</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="37">
+        <v>0.27</v>
+      </c>
+      <c r="H40" s="38">
+        <f t="shared" si="4"/>
+        <v>2.2331887603305787</v>
+      </c>
+      <c r="I40" s="39">
+        <f t="shared" si="4"/>
+        <v>2.3559852066115696</v>
+      </c>
+      <c r="J40" s="40">
+        <f t="shared" si="4"/>
+        <v>2.4816735537190087</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C41" s="6">
+        <f t="shared" si="1"/>
+        <v>3.5636363636363635</v>
+      </c>
+      <c r="D41" s="6">
+        <f t="shared" si="2"/>
+        <v>3.6909090909090909</v>
+      </c>
+      <c r="E41" s="11">
+        <f t="shared" si="3"/>
+        <v>3.8181818181818179</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="41">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H41" s="34">
+        <f t="shared" si="4"/>
+        <v>2.3605887603305784</v>
+      </c>
+      <c r="I41" s="35">
+        <f t="shared" si="4"/>
+        <v>2.4910988429752066</v>
+      </c>
+      <c r="J41" s="36">
+        <f t="shared" si="4"/>
+        <v>2.6247190082644622</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C42" s="6">
+        <f t="shared" si="1"/>
+        <v>3.6909090909090905</v>
+      </c>
+      <c r="D42" s="6">
+        <f t="shared" si="2"/>
+        <v>3.8227272727272723</v>
+      </c>
+      <c r="E42" s="11">
+        <f t="shared" si="3"/>
+        <v>3.9545454545454537</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="37">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H42" s="38">
+        <f t="shared" si="4"/>
+        <v>2.4910988429752061</v>
+      </c>
+      <c r="I42" s="39">
+        <f t="shared" si="4"/>
+        <v>2.6295486776859498</v>
+      </c>
+      <c r="J42" s="40">
+        <f t="shared" si="4"/>
+        <v>2.7713347107438007</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="C43" s="6">
+        <f t="shared" si="1"/>
+        <v>3.8181818181818179</v>
+      </c>
+      <c r="D43" s="6">
+        <f t="shared" si="2"/>
+        <v>3.9545454545454537</v>
+      </c>
+      <c r="E43" s="11">
+        <f t="shared" si="3"/>
+        <v>4.0909090909090908</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="41">
+        <v>0.3</v>
+      </c>
+      <c r="H43" s="34">
+        <f t="shared" si="4"/>
+        <v>2.6247190082644622</v>
+      </c>
+      <c r="I43" s="35">
+        <f t="shared" si="4"/>
+        <v>2.7713347107438007</v>
+      </c>
+      <c r="J43" s="36">
+        <f t="shared" si="4"/>
+        <v>2.9215206611570248</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="C44" s="6">
+        <f t="shared" si="1"/>
+        <v>3.9454545454545449</v>
+      </c>
+      <c r="D44" s="6">
+        <f t="shared" si="2"/>
+        <v>4.086363636363636</v>
+      </c>
+      <c r="E44" s="11">
+        <f t="shared" si="3"/>
+        <v>4.2272727272727275</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="37">
+        <v>0.31</v>
+      </c>
+      <c r="H44" s="38">
+        <f t="shared" si="4"/>
+        <v>2.7614492561983464</v>
+      </c>
+      <c r="I44" s="39">
+        <f t="shared" si="4"/>
+        <v>2.9164569421487596</v>
+      </c>
+      <c r="J44" s="40">
+        <f t="shared" si="4"/>
+        <v>3.0752768595041324</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="C45" s="6">
+        <f t="shared" si="1"/>
+        <v>4.0727272727272732</v>
+      </c>
+      <c r="D45" s="6">
+        <f t="shared" si="2"/>
+        <v>4.2181818181818178</v>
+      </c>
+      <c r="E45" s="11">
+        <f t="shared" si="3"/>
+        <v>4.3636363636363633</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="41">
+        <v>0.32</v>
+      </c>
+      <c r="H45" s="34">
+        <f t="shared" si="4"/>
+        <v>2.9012895867768598</v>
+      </c>
+      <c r="I45" s="35">
+        <f t="shared" si="4"/>
+        <v>3.0649153719008262</v>
+      </c>
+      <c r="J45" s="36">
+        <f t="shared" si="4"/>
+        <v>3.2326033057851236</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="C46" s="6">
+        <f t="shared" si="1"/>
+        <v>4.2</v>
+      </c>
+      <c r="D46" s="6">
+        <f t="shared" si="2"/>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="E46" s="11">
+        <f t="shared" si="3"/>
+        <v>4.5</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="37">
+        <v>0.33</v>
+      </c>
+      <c r="H46" s="38">
+        <f t="shared" si="4"/>
+        <v>3.0442399999999998</v>
+      </c>
+      <c r="I46" s="39">
+        <f t="shared" si="4"/>
+        <v>3.2167099999999995</v>
+      </c>
+      <c r="J46" s="40">
+        <f t="shared" si="4"/>
+        <v>3.3935</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="C47" s="6">
+        <f t="shared" si="1"/>
+        <v>4.3272727272727272</v>
+      </c>
+      <c r="D47" s="6">
+        <f t="shared" si="2"/>
+        <v>4.4818181818181824</v>
+      </c>
+      <c r="E47" s="11">
+        <f t="shared" si="3"/>
+        <v>4.6363636363636367</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="41">
+        <v>0.34</v>
+      </c>
+      <c r="H47" s="34">
+        <f t="shared" si="4"/>
+        <v>3.1903004958677683</v>
+      </c>
+      <c r="I47" s="35">
+        <f t="shared" si="4"/>
+        <v>3.3718408264462814</v>
+      </c>
+      <c r="J47" s="36">
+        <f t="shared" si="4"/>
+        <v>3.5579669421487607</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="C48" s="6">
+        <f t="shared" si="1"/>
+        <v>4.4545454545454541</v>
+      </c>
+      <c r="D48" s="6">
+        <f t="shared" si="2"/>
+        <v>4.6136363636363624</v>
+      </c>
+      <c r="E48" s="11">
+        <f t="shared" si="3"/>
+        <v>4.7727272727272725</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="37">
+        <v>0.35</v>
+      </c>
+      <c r="H48" s="38">
+        <f t="shared" si="4"/>
+        <v>3.3394710743801648</v>
+      </c>
+      <c r="I48" s="39">
+        <f t="shared" si="4"/>
+        <v>3.5303078512396682</v>
+      </c>
+      <c r="J48" s="40">
+        <f t="shared" si="4"/>
+        <v>3.7260041322314046</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="C49" s="6">
+        <f t="shared" si="1"/>
+        <v>4.5818181818181811</v>
+      </c>
+      <c r="D49" s="6">
+        <f t="shared" si="2"/>
+        <v>4.7454545454545451</v>
+      </c>
+      <c r="E49" s="11">
+        <f t="shared" si="3"/>
+        <v>4.9090909090909083</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="41">
+        <v>0.36</v>
+      </c>
+      <c r="H49" s="34">
+        <f t="shared" si="4"/>
+        <v>3.4917517355371888</v>
+      </c>
+      <c r="I49" s="35">
+        <f t="shared" si="4"/>
+        <v>3.6921110743801648</v>
+      </c>
+      <c r="J49" s="36">
+        <f t="shared" si="4"/>
+        <v>3.8976115702479333</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="8">
+        <v>0.37</v>
+      </c>
+      <c r="C50" s="6">
+        <f t="shared" si="1"/>
+        <v>4.7090909090909081</v>
+      </c>
+      <c r="D50" s="6">
+        <f t="shared" si="2"/>
+        <v>4.877272727272727</v>
+      </c>
+      <c r="E50" s="11">
+        <f t="shared" si="3"/>
+        <v>5.045454545454545</v>
+      </c>
+      <c r="G50" s="37">
+        <v>0.37</v>
+      </c>
+      <c r="H50" s="38">
+        <f t="shared" si="4"/>
+        <v>3.6471424793388416</v>
+      </c>
+      <c r="I50" s="39">
+        <f t="shared" si="4"/>
+        <v>3.8572504958677682</v>
+      </c>
+      <c r="J50" s="40">
+        <f t="shared" si="4"/>
+        <v>4.0727892561983472</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="8">
+        <v>0.38</v>
+      </c>
+      <c r="C51" s="6">
+        <f t="shared" si="1"/>
+        <v>4.836363636363636</v>
+      </c>
+      <c r="D51" s="6">
+        <f t="shared" si="2"/>
+        <v>5.0090909090909088</v>
+      </c>
+      <c r="E51" s="11">
+        <f t="shared" si="3"/>
+        <v>5.1818181818181817</v>
+      </c>
+      <c r="G51" s="41">
+        <v>0.38</v>
+      </c>
+      <c r="H51" s="34">
+        <f t="shared" si="4"/>
+        <v>3.8056433057851233</v>
+      </c>
+      <c r="I51" s="35">
+        <f t="shared" si="4"/>
+        <v>4.0257261157024793</v>
+      </c>
+      <c r="J51" s="36">
+        <f t="shared" si="4"/>
+        <v>4.2515371900826446</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="C52" s="6">
+        <f t="shared" si="1"/>
+        <v>4.963636363636363</v>
+      </c>
+      <c r="D52" s="6">
+        <f t="shared" si="2"/>
+        <v>5.1409090909090907</v>
+      </c>
+      <c r="E52" s="11">
+        <f t="shared" si="3"/>
+        <v>5.3181818181818183</v>
+      </c>
+      <c r="G52" s="42">
+        <v>0.39</v>
+      </c>
+      <c r="H52" s="38">
+        <f t="shared" si="4"/>
+        <v>3.9672542148760321</v>
+      </c>
+      <c r="I52" s="39">
+        <f t="shared" si="4"/>
+        <v>4.1975379338842975</v>
+      </c>
+      <c r="J52" s="40">
+        <f t="shared" si="4"/>
+        <v>4.4338553719008269</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C53" s="10">
+        <f t="shared" si="1"/>
+        <v>5.0909090909090908</v>
+      </c>
+      <c r="D53" s="10">
+        <f t="shared" si="2"/>
+        <v>5.2727272727272734</v>
+      </c>
+      <c r="E53" s="12">
+        <f t="shared" si="3"/>
+        <v>5.4545454545454541</v>
+      </c>
+      <c r="G53" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="H53" s="44">
+        <f t="shared" si="4"/>
+        <v>4.1319752066115703</v>
+      </c>
+      <c r="I53" s="45">
+        <f t="shared" si="4"/>
+        <v>4.3726859504132243</v>
+      </c>
+      <c r="J53" s="46">
+        <f t="shared" si="4"/>
+        <v>4.6197438016528922</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="G13:J13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup scale="86" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>